<commit_message>
updating column to just have state name
</commit_message>
<xml_diff>
--- a/Rainfall Data Sets/Clean_Rainfall_By_State.xlsx
+++ b/Rainfall Data Sets/Clean_Rainfall_By_State.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franz/Desktop/Data Visualisation 2/Rainfall Data Sets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051F9A8E-E34C-084D-9F29-A2F189E19EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EA4CD8-00EF-AE41-8C5C-59F751DB1F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21040" yWindow="5160" windowWidth="27500" windowHeight="18220" xr2:uid="{F293E0A7-5C67-3D4D-B8CF-2550A95850C8}"/>
   </bookViews>
@@ -44,28 +44,28 @@
     <t>Average Precipitation (millimetres)</t>
   </si>
   <si>
-    <t>South Australia (Adelaide)</t>
-  </si>
-  <si>
-    <t>Queensland (Brisbane)</t>
-  </si>
-  <si>
-    <t>ACT (Canberra)</t>
-  </si>
-  <si>
-    <t>Northern Territory (Darwin)</t>
-  </si>
-  <si>
-    <t>Tasmania (Hobart)</t>
-  </si>
-  <si>
-    <t>Victoria (Melbourne)</t>
-  </si>
-  <si>
-    <t>Western Australia (Perth)</t>
-  </si>
-  <si>
-    <t>New South Wales (Sydney)</t>
+    <t>South Australia</t>
+  </si>
+  <si>
+    <t>Queensland</t>
+  </si>
+  <si>
+    <t>Australian Capital Territory</t>
+  </si>
+  <si>
+    <t>Northern Territory</t>
+  </si>
+  <si>
+    <t>Tasmania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victoria </t>
+  </si>
+  <si>
+    <t>Western Australia</t>
+  </si>
+  <si>
+    <t>New South Wales</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>